<commit_message>
Time displacement, same day, day banned constrictions done.
</commit_message>
<xml_diff>
--- a/files/pruebas/v6_sinFechas.xlsx
+++ b/files/pruebas/v6_sinFechas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\TfgProject\files\pruebas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9952EB8B-01FA-4167-A1F5-36F1D65090B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECA2450A-4DDF-48D3-8824-72D2663B3FE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="planificación" sheetId="2" r:id="rId1"/>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="894" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="914" uniqueCount="383">
   <si>
     <t>ID</t>
   </si>
@@ -1252,6 +1252,12 @@
   </si>
   <si>
     <t>TD</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>DB</t>
   </si>
 </sst>
 </file>
@@ -1751,7 +1757,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -1844,11 +1850,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2314,7 +2321,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+    <sheetView topLeftCell="B4" workbookViewId="0">
       <selection activeCell="O65" sqref="O65"/>
     </sheetView>
   </sheetViews>
@@ -2404,16 +2411,16 @@
       <c r="N5" s="73" t="s">
         <v>356</v>
       </c>
-      <c r="O5" s="93" t="s">
+      <c r="O5" s="92" t="s">
         <v>281</v>
       </c>
-      <c r="P5" s="93" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="92" t="s">
+      <c r="P5" s="92" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="94" t="s">
         <v>299</v>
       </c>
-      <c r="R5" s="92"/>
+      <c r="R5" s="94"/>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="75">
@@ -6461,10 +6468,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AC83AD5-6F52-41B7-9F54-B20EA3E13FEF}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39:B40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6472,7 +6479,7 @@
     <col min="2" max="3" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>380</v>
       </c>
@@ -6486,7 +6493,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>380</v>
       </c>
@@ -6500,7 +6507,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>380</v>
       </c>
@@ -6514,49 +6521,276 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>380</v>
       </c>
       <c r="B4">
         <v>60</v>
       </c>
-      <c r="C4" s="94">
+      <c r="C4" s="93">
         <v>15</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>380</v>
       </c>
       <c r="B5">
         <v>24</v>
       </c>
-      <c r="C5" s="94">
+      <c r="C5" s="93">
         <v>38</v>
       </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>380</v>
+      </c>
+      <c r="B6">
+        <v>13</v>
+      </c>
+      <c r="C6" s="93">
+        <v>38</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>381</v>
+      </c>
+      <c r="B7">
+        <v>46</v>
+      </c>
+      <c r="C7" s="93">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>381</v>
+      </c>
+      <c r="B8">
+        <v>34</v>
+      </c>
+      <c r="C8" s="93">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>381</v>
+      </c>
+      <c r="B9">
+        <v>47</v>
+      </c>
+      <c r="C9" s="93">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>382</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10" s="79">
+        <v>44361</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>382</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11" s="14">
+        <v>44362</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>382</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12" s="14">
+        <v>44363</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>382</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13" s="14">
+        <v>44365</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>382</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14" s="14">
+        <v>44368</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>382</v>
+      </c>
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15" s="14">
+        <v>44369</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>382</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16" s="14">
+        <v>44370</v>
+      </c>
+      <c r="E16" s="95"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>382</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="C17" s="14">
+        <v>44371</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>382</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="C18" s="14">
+        <v>44372</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>382</v>
+      </c>
+      <c r="B19">
+        <v>3</v>
+      </c>
+      <c r="C19" s="14">
+        <v>44375</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>382</v>
+      </c>
+      <c r="B20">
+        <v>3</v>
+      </c>
+      <c r="C20" s="14">
+        <v>44376</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>382</v>
+      </c>
+      <c r="B21">
+        <v>3</v>
+      </c>
+      <c r="C21" s="14">
+        <v>44377</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>382</v>
+      </c>
+      <c r="B22">
+        <v>3</v>
+      </c>
+      <c r="C22" s="14">
+        <v>44378</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>382</v>
+      </c>
+      <c r="B23">
+        <v>3</v>
+      </c>
+      <c r="C23" s="14">
+        <v>44379</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>382</v>
+      </c>
+      <c r="B24">
+        <v>3</v>
+      </c>
+      <c r="C24" s="14">
+        <v>44382</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>382</v>
+      </c>
+      <c r="B25">
+        <v>3</v>
+      </c>
+      <c r="C25" s="14">
+        <v>44383</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B1">
-    <cfRule type="expression" dxfId="4" priority="4">
+  <conditionalFormatting sqref="B1 C10:C25">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>$Q1=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="expression" dxfId="3" priority="3">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>$Q2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>$Q3=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3:C5">
-    <cfRule type="expression" dxfId="1" priority="1">
+  <conditionalFormatting sqref="C3:C9">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>$Q3=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6569,7 +6803,7 @@
   <dimension ref="A1:A17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection sqref="A1:A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>